<commit_message>
Buzzer round details added
</commit_message>
<xml_diff>
--- a/public/inputQuiz/Template.xlsx
+++ b/public/inputQuiz/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\QUIZ\quiz-app\public\inputQuiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12979348-0B46-4A4E-AF08-F92553896874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFB460C-2A1C-44B2-9D6B-FE6080849AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0C723560-6435-4BE6-81A6-ADB39D116BD3}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="440">
   <si>
     <t>Q1</t>
   </si>
@@ -104,48 +104,15 @@
     <t>Answers</t>
   </si>
   <si>
-    <t>उक्त चित्र को पहचाने?</t>
-  </si>
-  <si>
-    <t>सेंट्रल विस्टा</t>
-  </si>
-  <si>
-    <t>यह कहाँ स्थित है? (शहर)</t>
-  </si>
-  <si>
-    <t>नई दिल्ली</t>
-  </si>
-  <si>
-    <t>सेंट्रल विस्टा की आधारशिला किसने रखी?</t>
-  </si>
-  <si>
-    <t>प्रधानमंत्री श्री नरेन्द्र मोदी (10 दिसम्बर 2020)</t>
-  </si>
-  <si>
     <t>उक्त चित्र किस महापुरुष का है?</t>
   </si>
   <si>
-    <t>यह उत्तराखण्ड राज्य के किस जनपद से हैं?</t>
-  </si>
-  <si>
-    <t>1957 में इन्हें कौन सा सर्वोच्च सम्मान दिया गया?</t>
-  </si>
-  <si>
-    <t>श्री गोविन्द वल्लभ पन्त</t>
-  </si>
-  <si>
     <t>अल्मोड़ा</t>
   </si>
   <si>
-    <t>भारत रत्न</t>
-  </si>
-  <si>
     <t>उक्त लोगो किस संस्था का है?</t>
   </si>
   <si>
-    <t>बी0 सी0 सी0 आई0 (Board of Control for Cricket in India)</t>
-  </si>
-  <si>
     <t>Marks</t>
   </si>
   <si>
@@ -188,9 +155,6 @@
     <t>Negative Marking</t>
   </si>
   <si>
-    <t>थॉमस कप</t>
-  </si>
-  <si>
     <t>1947 में जब भारत आज़ाद हुआ, उस समय ब्रिटेन के प्रधानमंत्री कौन थे?</t>
   </si>
   <si>
@@ -230,9 +194,6 @@
     <t>नीलम संजीवा रेड्डी</t>
   </si>
   <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual_Team1.m4v</t>
-  </si>
-  <si>
     <t>ग्लास्गो</t>
   </si>
   <si>
@@ -245,235 +206,10 @@
     <t>टोक्यो</t>
   </si>
   <si>
-    <t>कर्नाटक</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team1_Pic1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team1_Pic2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team1_Pic3.jpg</t>
-  </si>
-  <si>
-    <t>उक्त चित्र को पहचाने?उक्त स्मारक क नाम बताएं?</t>
-  </si>
-  <si>
-    <t>नेशनल वार मेमोरियल</t>
-  </si>
-  <si>
-    <t>यह स्मारक किस शहर में स्थित है?</t>
-  </si>
-  <si>
-    <t>इसके पूर्व स्मारक की लौ दिल्ली में कहाँ प्रज्जवलित होती थी?</t>
-  </si>
-  <si>
-    <t>इंडिया गेट</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team2_Pic1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team2_Pic2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team2_Pic3.jpg</t>
-  </si>
-  <si>
-    <t>उक्त चित्र किसका है?</t>
-  </si>
-  <si>
-    <t>लक्ष्य सेन</t>
-  </si>
-  <si>
-    <t>लक्ष्य सेन मूलतः उत्तराखण्ड के किस जनपद के हैं?</t>
-  </si>
-  <si>
-    <t>2022 में इनके सहयोग से भारत ने इंडोनेशिया में कौन सा ख़िताब जीता?</t>
-  </si>
-  <si>
-    <t>कॉमन वेल्थ</t>
-  </si>
-  <si>
-    <t>उक्त प्रतिमा किसकी है?</t>
-  </si>
-  <si>
-    <t>नेता जी सुभाष चन्द्र बोस</t>
-  </si>
-  <si>
-    <t>नई दिल्ली में किस स्थान पर स्थापित की गयी है?</t>
-  </si>
-  <si>
-    <t>उक्त प्रतिमा के मूर्तिकार का नाम बताएं?</t>
-  </si>
-  <si>
-    <t>श्री अरुण योगिराज</t>
-  </si>
-  <si>
-    <t>डा0 सी0 वी0 रमन</t>
-  </si>
-  <si>
-    <t>इन्हें किस सन में भौतिकी का नोबेल पुरस्कार दिया गया?</t>
-  </si>
-  <si>
-    <t>1930 में.</t>
-  </si>
-  <si>
-    <t>यह मूलतः किस राज्य के थे?</t>
-  </si>
-  <si>
-    <t>चेन्नई</t>
-  </si>
-  <si>
-    <t>उक्त लोगो पहचाने?</t>
-  </si>
-  <si>
-    <t>IAEA (International Atomic Energy Agency)</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team3_Pic1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team3_Pic2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team3_Pic3.jpg</t>
-  </si>
-  <si>
-    <t>उक्त प्रतिमा किस संत की है?</t>
-  </si>
-  <si>
-    <t>आदि गुरु शंकराचार्य</t>
-  </si>
-  <si>
-    <t>यह प्रतिमा कहाँ स्थापित है?</t>
-  </si>
-  <si>
-    <t>केदारनाथ (रुद्रप्रयाग)</t>
-  </si>
-  <si>
-    <t>इस प्रतिमा के मुख्य मूर्तिकार कौन थे?</t>
-  </si>
-  <si>
-    <t>योगिराज शिल्पी</t>
-  </si>
-  <si>
-    <t>उक्त चित्र किस व्यक्ति का है?</t>
-  </si>
-  <si>
-    <t>CDS अनिल चौहान</t>
-  </si>
-  <si>
-    <t>सी0दी0एस0 बनने से पूर्व सेना के किस पद से सेवानिवृत्त हुए थे?</t>
-  </si>
-  <si>
-    <t>लेफ्टिनेंट जनरल</t>
-  </si>
-  <si>
-    <t>मूलतः उत्तराखण्ड के किस जनपद से हैं?</t>
-  </si>
-  <si>
     <t>पौड़ी गढ़वाल</t>
   </si>
   <si>
-    <t>अंतर्राष्ट्रीय योग दिवस</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team4_Pic1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team4_Pic2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team4_Pic3.jpg</t>
-  </si>
-  <si>
-    <t>उक्त चित्र किस मंदिर का है?</t>
-  </si>
-  <si>
-    <t>राम मंदिर (अयोध्या)</t>
-  </si>
-  <si>
-    <t>इस मंदिर के वास्तुकार का नाम बताएं?</t>
-  </si>
-  <si>
-    <t>चन्द्र कान्त सोमपुरा</t>
-  </si>
-  <si>
-    <t>प्रधानमंत्री नरेंद्र मोदी जी ने इसका शिलान्यास किस तिथि को किया?</t>
-  </si>
-  <si>
-    <t>5 अगस्त को</t>
-  </si>
-  <si>
-    <t>एस० जयशंकर</t>
-  </si>
-  <si>
-    <t>यह वर्तमान में किस पद पर हैं?</t>
-  </si>
-  <si>
-    <t>भारत केविदेश मंत्री</t>
-  </si>
-  <si>
-    <t>इनका पूरा नाम बताएं?</t>
-  </si>
-  <si>
-    <t>सुब्रह्मण्यम जयशंकर</t>
-  </si>
-  <si>
-    <t>भारतीय वायु सेना</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team5_Pic1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team5_Pic2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team5_Pic3.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team6_Pic1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team6_Pic2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\Visual\Visual_Team6_Pic3.jpg</t>
-  </si>
-  <si>
     <t>उक्त ईमारत का नाम बताएं?</t>
-  </si>
-  <si>
-    <t>मैसूर महल</t>
-  </si>
-  <si>
-    <t>यह किस राज्य में स्थित है?</t>
-  </si>
-  <si>
-    <t>इसका निर्माण किस वंश ने करवाया?</t>
-  </si>
-  <si>
-    <t>वाडियार वंश</t>
-  </si>
-  <si>
-    <t>होमी जहाँगीर भाभा</t>
-  </si>
-  <si>
-    <t>इन्होने विज्ञान के किस क्षेत्र में कार्य किया?</t>
-  </si>
-  <si>
-    <t>नाभिकीय/परमाणु ऊर्जा</t>
-  </si>
-  <si>
-    <t>भाभा जी का निधन विमान दुर्घटना में किस सन में हुआ?</t>
-  </si>
-  <si>
-    <t>1966 में.</t>
-  </si>
-  <si>
-    <t>ILO (International Labour Organization)</t>
   </si>
   <si>
     <t xml:space="preserve">SUTTER </t>
@@ -1347,22 +1083,280 @@
     <t>धारा-370</t>
   </si>
   <si>
-    <t>E:\quiz-app\public\inputQuiz\MCQ\MCQ_Team1.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\MCQ\MCQ_Team2.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\MCQ\MCQ_Team3.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\MCQ\MCQ_Team4.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\MCQ\MCQ_Team5.jpg</t>
-  </si>
-  <si>
-    <t>E:\quiz-app\public\inputQuiz\MCQ\MCQ_Team6.jpg</t>
+    <t>..\public\inputQuiz\MCQ\MCQ_Team1.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\MCQ\MCQ_Team2.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\MCQ\MCQ_Team3.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\MCQ\MCQ_Team4.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\MCQ\MCQ_Team5.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\MCQ\MCQ_Team6.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team3_Pic2.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team3_Pic3.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team4_Pic1.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team5_Pic1.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team5_Pic2.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team6_Pic1.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team6_Pic3.jpg</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team1_Pic1.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team1_Pic2.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team1_Pic3.png</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team2_Pic1.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team2_Pic2.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team2_Pic3.png</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team3_Pic1.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team4_Pic2.png</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team4_Pic3.png</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team5_Pic3.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual\Visual_Team6_Pic2.webp</t>
+  </si>
+  <si>
+    <t>..\public\inputQuiz\Visual_Team1.m4v</t>
+  </si>
+  <si>
+    <t>डॉ. एम. एस. स्वामीनाथन</t>
+  </si>
+  <si>
+    <t>अल-अक्सा मस्जिद</t>
+  </si>
+  <si>
+    <t>चेन्नई, तमिलनाडु</t>
+  </si>
+  <si>
+    <t>कृषि वैज्ञानिक</t>
+  </si>
+  <si>
+    <t>यह किस देश में स्थित है?</t>
+  </si>
+  <si>
+    <t>इज़राइल(यरूशलेम)</t>
+  </si>
+  <si>
+    <t>7-8 शताब्दी</t>
+  </si>
+  <si>
+    <t>ASEAN</t>
+  </si>
+  <si>
+    <t>इनका संबंध मूलतः किस राज्य से है?</t>
+  </si>
+  <si>
+    <t>इनका संबंध किस क्षेत्र से है?</t>
+  </si>
+  <si>
+    <t>उक्त इमारत किस शताब्दी के मध्य बनी?</t>
+  </si>
+  <si>
+    <t>उक्त चित्र किस महिला का है?</t>
+  </si>
+  <si>
+    <t>आशा पारेख</t>
+  </si>
+  <si>
+    <t>दादा साहेब फाल्के पुरस्कार</t>
+  </si>
+  <si>
+    <t>मुंबई</t>
+  </si>
+  <si>
+    <t>उत्तराखंड विधान सभा</t>
+  </si>
+  <si>
+    <t>यह किस शहर/जनपद में स्थित है?</t>
+  </si>
+  <si>
+    <t>गैरसैंण(चमोली)</t>
+  </si>
+  <si>
+    <t>9 जून 2014 को</t>
+  </si>
+  <si>
+    <t>उक्त लोगो किस का है?</t>
+  </si>
+  <si>
+    <t>एशियाई खेल हांग्जो (चीन)</t>
+  </si>
+  <si>
+    <t>इन्हें वर्तमान में कौनसा पुरस्कार मिला?</t>
+  </si>
+  <si>
+    <t>इनका जन्म किस शहर में हुआ?</t>
+  </si>
+  <si>
+    <t>गैरसैंण मे पहला विधानसभा सत्र कब हुआ?</t>
+  </si>
+  <si>
+    <t>उक्त चित्र किस खिलाड़ी का है?</t>
+  </si>
+  <si>
+    <t>रमेशबाबू प्रग्गनानंद</t>
+  </si>
+  <si>
+    <t>इनका संबंध किस खेल से है?</t>
+  </si>
+  <si>
+    <t>माउंट रशमोर राष्ट्रीय स्मारक</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>जॉर्ज वाशिंगटन, थॉमस जेफरसन, थियोडोर रूजवेल्ट और अब्राहम लिंकन</t>
+  </si>
+  <si>
+    <t>उक्त चित्र में अमेरिका के चारों राष्ट्रपति के नाम बताए?</t>
+  </si>
+  <si>
+    <t>प्रधानमंत्री जन आरोग्य योजना (PM-JAY)</t>
+  </si>
+  <si>
+    <t>उक्त चित्र किस का है?</t>
+  </si>
+  <si>
+    <t>भुवन चंद्र खंडूरी</t>
+  </si>
+  <si>
+    <t>भारतीय सेना के किस पद से सेवानिवृत्त हुए?</t>
+  </si>
+  <si>
+    <t>मेजर जनरल</t>
+  </si>
+  <si>
+    <t>उत्तराखंड के मुख्यमंत्री कब बने?</t>
+  </si>
+  <si>
+    <t>8 मार्च 2007</t>
+  </si>
+  <si>
+    <t>पैलेस ऑफ वेस्टमिन्स्टर</t>
+  </si>
+  <si>
+    <t>ब्रिटेन</t>
+  </si>
+  <si>
+    <t>वर्तमान में यहाँ ब्रिटेन का क्या है?</t>
+  </si>
+  <si>
+    <t>ब्रिटेन की संसद</t>
+  </si>
+  <si>
+    <t>उक्त झंडा किस देश का है?</t>
+  </si>
+  <si>
+    <t>इजराइल</t>
+  </si>
+  <si>
+    <t>मार्शल ऑफ द एयर फोर्स अर्जन सिंह</t>
+  </si>
+  <si>
+    <t>इन्होंने कौन से भारत पाकिस्तान युद्ध में प्रसिद्धि अर्जित की?</t>
+  </si>
+  <si>
+    <t>इनकी मृत्यु कब हुई?</t>
+  </si>
+  <si>
+    <t>16 सितम्बर 2017</t>
+  </si>
+  <si>
+    <t>उक्त मंदिर का नाम बताएं?</t>
+  </si>
+  <si>
+    <t>जागेश्वर धाम</t>
+  </si>
+  <si>
+    <t>ये उत्तराखंड के किस जनपद में स्थित है?</t>
+  </si>
+  <si>
+    <t>अल्मोडा</t>
+  </si>
+  <si>
+    <t>इसका निर्माण किस राजवंश ने कराया?</t>
+  </si>
+  <si>
+    <t>कत्यूरी राजवंश</t>
+  </si>
+  <si>
+    <t>यूरोपीय संघ</t>
+  </si>
+  <si>
+    <t>नरगिस सफ़ी मोहम्मदी</t>
+  </si>
+  <si>
+    <t>इनका संबंध किस देश से है?</t>
+  </si>
+  <si>
+    <t>ईरान</t>
+  </si>
+  <si>
+    <t>इन्हें 2023 में नोबल शांति पुरस्कार किस कार्य के लिए मिला?</t>
+  </si>
+  <si>
+    <t>मानवाधिकार कार्यकर्ता</t>
+  </si>
+  <si>
+    <t>अंकोरवाट मन्दिर</t>
+  </si>
+  <si>
+    <t>यह मंदिर किस देश में स्थित है?</t>
+  </si>
+  <si>
+    <t>कम्बोडिया</t>
+  </si>
+  <si>
+    <t>यह मंदिर किस भगवान का है?</t>
+  </si>
+  <si>
+    <t>विष्णु भगवान</t>
+  </si>
+  <si>
+    <t>उक्त लोगो(वस्तु) का नाम बताइए?</t>
+  </si>
+  <si>
+    <t>सेंगोल</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1777,6 +1771,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2096,10 +2096,10 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2108,11 +2108,11 @@
     <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="98.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2145,7 +2145,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2156,19 +2156,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>256</v>
+        <v>168</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>260</v>
+        <v>172</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>279</v>
+        <v>191</v>
       </c>
       <c r="H2" s="5">
         <v>30</v>
@@ -2186,19 +2186,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>207</v>
+        <v>119</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>261</v>
+        <v>173</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>280</v>
+        <v>192</v>
       </c>
       <c r="H3" s="7">
         <v>30</v>
@@ -2216,19 +2216,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>208</v>
+        <v>120</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>258</v>
+        <v>170</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>262</v>
+        <v>174</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>281</v>
+        <v>193</v>
       </c>
       <c r="H4" s="7">
         <v>30</v>
@@ -2246,25 +2246,25 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>209</v>
+        <v>121</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>259</v>
+        <v>171</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>263</v>
+        <v>175</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>282</v>
+        <v>194</v>
       </c>
       <c r="H5" s="7">
         <v>30</v>
       </c>
       <c r="I5" s="53" t="s">
-        <v>436</v>
+        <v>348</v>
       </c>
       <c r="J5" s="8">
         <v>5</v>
@@ -2278,7 +2278,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="D6" s="10">
         <v>5</v>
@@ -2308,19 +2308,19 @@
         <v>0</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>284</v>
+        <v>196</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>291</v>
+        <v>203</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>264</v>
+        <v>176</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>283</v>
+        <v>195</v>
       </c>
       <c r="H7" s="5">
         <v>30</v>
@@ -2338,19 +2338,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>210</v>
+        <v>122</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>225</v>
+        <v>137</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>240</v>
+        <v>152</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
       <c r="H8" s="7">
         <v>30</v>
@@ -2368,19 +2368,19 @@
         <v>2</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>184</v>
+        <v>96</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>211</v>
+        <v>123</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>241</v>
+        <v>153</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>265</v>
+        <v>177</v>
       </c>
       <c r="H9" s="7">
         <v>30</v>
@@ -2398,25 +2398,25 @@
         <v>3</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>185</v>
+        <v>97</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>212</v>
+        <v>124</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>227</v>
+        <v>139</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>242</v>
+        <v>154</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>266</v>
+        <v>178</v>
       </c>
       <c r="H10" s="7">
         <v>30</v>
       </c>
       <c r="I10" s="53" t="s">
-        <v>437</v>
+        <v>349</v>
       </c>
       <c r="J10" s="8">
         <v>5</v>
@@ -2430,19 +2430,19 @@
         <v>4</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>186</v>
+        <v>98</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>213</v>
+        <v>125</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>228</v>
+        <v>140</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>243</v>
+        <v>155</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>267</v>
+        <v>179</v>
       </c>
       <c r="H11" s="10">
         <v>60</v>
@@ -2460,19 +2460,19 @@
         <v>0</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>187</v>
+        <v>99</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>214</v>
+        <v>126</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>292</v>
+        <v>204</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>244</v>
+        <v>156</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>268</v>
+        <v>180</v>
       </c>
       <c r="H12" s="5">
         <v>30</v>
@@ -2490,19 +2490,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>188</v>
+        <v>100</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>285</v>
+        <v>197</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>293</v>
+        <v>205</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>298</v>
+        <v>210</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>303</v>
+        <v>215</v>
       </c>
       <c r="H13" s="7">
         <v>30</v>
@@ -2520,19 +2520,19 @@
         <v>2</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>215</v>
+        <v>127</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>229</v>
+        <v>141</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>269</v>
+        <v>181</v>
       </c>
       <c r="H14" s="7">
         <v>30</v>
@@ -2550,25 +2550,25 @@
         <v>3</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>190</v>
+        <v>102</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>230</v>
+        <v>142</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>246</v>
+        <v>158</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>270</v>
+        <v>182</v>
       </c>
       <c r="H15" s="7">
         <v>30</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>438</v>
+        <v>350</v>
       </c>
       <c r="J15" s="8">
         <v>5</v>
@@ -2582,7 +2582,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="D16" s="10">
         <v>45</v>
@@ -2612,19 +2612,19 @@
         <v>0</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>217</v>
+        <v>129</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>231</v>
+        <v>143</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>247</v>
+        <v>159</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>271</v>
+        <v>183</v>
       </c>
       <c r="H17" s="5">
         <v>30</v>
@@ -2642,19 +2642,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>286</v>
+        <v>198</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>232</v>
+        <v>144</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>248</v>
+        <v>160</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>272</v>
+        <v>184</v>
       </c>
       <c r="H18" s="7">
         <v>30</v>
@@ -2672,19 +2672,19 @@
         <v>2</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="H19" s="7">
         <v>30</v>
@@ -2702,25 +2702,25 @@
         <v>3</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>195</v>
+        <v>107</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>218</v>
+        <v>130</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>233</v>
+        <v>145</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>249</v>
+        <v>161</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>273</v>
+        <v>185</v>
       </c>
       <c r="H20" s="7">
         <v>30</v>
       </c>
       <c r="I20" s="53" t="s">
-        <v>439</v>
+        <v>351</v>
       </c>
       <c r="J20" s="8">
         <v>5</v>
@@ -2734,19 +2734,19 @@
         <v>4</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>205</v>
+        <v>117</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>299</v>
+        <v>211</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="H21" s="10">
         <v>60</v>
@@ -2764,19 +2764,19 @@
         <v>0</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>196</v>
+        <v>108</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>219</v>
+        <v>131</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>234</v>
+        <v>146</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>274</v>
+        <v>186</v>
       </c>
       <c r="H22" s="5">
         <v>30</v>
@@ -2794,19 +2794,19 @@
         <v>1</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>197</v>
+        <v>109</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>287</v>
+        <v>199</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>294</v>
+        <v>206</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>300</v>
+        <v>212</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>304</v>
+        <v>216</v>
       </c>
       <c r="H23" s="7">
         <v>30</v>
@@ -2824,19 +2824,19 @@
         <v>2</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>198</v>
+        <v>110</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>288</v>
+        <v>200</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>295</v>
+        <v>207</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>301</v>
+        <v>213</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>305</v>
+        <v>217</v>
       </c>
       <c r="H24" s="7">
         <v>30</v>
@@ -2854,25 +2854,25 @@
         <v>3</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>190</v>
+        <v>102</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>220</v>
+        <v>132</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>296</v>
+        <v>208</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>250</v>
+        <v>162</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>306</v>
+        <v>218</v>
       </c>
       <c r="H25" s="7">
         <v>30</v>
       </c>
       <c r="I25" s="53" t="s">
-        <v>440</v>
+        <v>352</v>
       </c>
       <c r="J25" s="8">
         <v>5</v>
@@ -2886,19 +2886,19 @@
         <v>4</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>289</v>
+        <v>201</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>297</v>
+        <v>209</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>302</v>
+        <v>214</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>302</v>
+        <v>214</v>
       </c>
       <c r="H26" s="10">
         <v>60</v>
@@ -2916,19 +2916,19 @@
         <v>0</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>221</v>
+        <v>133</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>235</v>
+        <v>147</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>251</v>
+        <v>163</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>275</v>
+        <v>187</v>
       </c>
       <c r="H27" s="5">
         <v>30</v>
@@ -2946,19 +2946,19 @@
         <v>1</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>201</v>
+        <v>113</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>222</v>
+        <v>134</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>236</v>
+        <v>148</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>252</v>
+        <v>164</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>276</v>
+        <v>188</v>
       </c>
       <c r="H28" s="7">
         <v>30</v>
@@ -2976,19 +2976,19 @@
         <v>2</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>202</v>
+        <v>114</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>223</v>
+        <v>135</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>237</v>
+        <v>149</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>253</v>
+        <v>165</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>307</v>
+        <v>219</v>
       </c>
       <c r="H29" s="7">
         <v>30</v>
@@ -3006,25 +3006,25 @@
         <v>3</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>203</v>
+        <v>115</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>290</v>
+        <v>202</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>238</v>
+        <v>150</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>254</v>
+        <v>166</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>277</v>
+        <v>189</v>
       </c>
       <c r="H30" s="7">
         <v>30</v>
       </c>
       <c r="I30" s="53" t="s">
-        <v>441</v>
+        <v>353</v>
       </c>
       <c r="J30" s="8">
         <v>5</v>
@@ -3038,19 +3038,19 @@
         <v>4</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>239</v>
+        <v>151</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>255</v>
+        <v>167</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>278</v>
+        <v>190</v>
       </c>
       <c r="H31" s="10">
         <v>60</v>
@@ -3078,45 +3078,45 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>38</v>
+      <c r="H1" s="21" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3130,13 +3130,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>373</v>
       </c>
       <c r="E2" s="5">
         <v>15</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>72</v>
+        <v>361</v>
       </c>
       <c r="G2" s="5">
         <v>15</v>
@@ -3149,22 +3149,22 @@
       <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="C3" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>375</v>
+      </c>
+      <c r="E3" s="59">
         <v>15</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="7">
+        <v>361</v>
+      </c>
+      <c r="G3" s="59">
         <v>15</v>
       </c>
       <c r="H3" s="8">
@@ -3175,22 +3175,22 @@
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="C4" s="59" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="E4" s="59">
         <v>15</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="7">
+        <v>361</v>
+      </c>
+      <c r="G4" s="59">
         <v>15</v>
       </c>
       <c r="H4" s="8">
@@ -3201,22 +3201,22 @@
       <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="C5" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>374</v>
+      </c>
+      <c r="E5" s="59">
         <v>15</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="7">
+        <v>362</v>
+      </c>
+      <c r="G5" s="59">
         <v>15</v>
       </c>
       <c r="H5" s="8">
@@ -3227,22 +3227,22 @@
       <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="C6" s="59" t="s">
+        <v>377</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>378</v>
+      </c>
+      <c r="E6" s="59">
         <v>15</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="7">
+        <v>362</v>
+      </c>
+      <c r="G6" s="59">
         <v>15</v>
       </c>
       <c r="H6" s="8">
@@ -3253,22 +3253,22 @@
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="C7" s="59" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>379</v>
+      </c>
+      <c r="E7" s="59">
         <v>15</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="7">
+        <v>362</v>
+      </c>
+      <c r="G7" s="59">
         <v>15</v>
       </c>
       <c r="H7" s="8">
@@ -3276,28 +3276,28 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="7">
-        <v>15</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="7">
-        <v>15</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="C8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" s="10">
+        <v>15</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="G8" s="10">
+        <v>15</v>
+      </c>
+      <c r="H8" s="11">
         <v>10</v>
       </c>
     </row>
@@ -3309,16 +3309,16 @@
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>75</v>
+        <v>384</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>76</v>
+        <v>385</v>
       </c>
       <c r="E9" s="5">
         <v>15</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>80</v>
+        <v>364</v>
       </c>
       <c r="G9" s="5">
         <v>15</v>
@@ -3331,22 +3331,22 @@
       <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="C10" s="59" t="s">
+        <v>394</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="E10" s="59">
         <v>15</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="7">
+        <v>364</v>
+      </c>
+      <c r="G10" s="59">
         <v>15</v>
       </c>
       <c r="H10" s="8">
@@ -3357,22 +3357,22 @@
       <c r="A11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="C11" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>387</v>
+      </c>
+      <c r="E11" s="59">
         <v>15</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="7">
+        <v>364</v>
+      </c>
+      <c r="G11" s="59">
         <v>15</v>
       </c>
       <c r="H11" s="8">
@@ -3383,22 +3383,22 @@
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="C12" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>388</v>
+      </c>
+      <c r="E12" s="59">
         <v>15</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="7">
+        <v>365</v>
+      </c>
+      <c r="G12" s="59">
         <v>15</v>
       </c>
       <c r="H12" s="8">
@@ -3409,22 +3409,22 @@
       <c r="A13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="59" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="7">
+        <v>389</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>390</v>
+      </c>
+      <c r="E13" s="59">
         <v>15</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="7">
+        <v>365</v>
+      </c>
+      <c r="G13" s="59">
         <v>15</v>
       </c>
       <c r="H13" s="8">
@@ -3435,22 +3435,22 @@
       <c r="A14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="C14" s="59" t="s">
+        <v>396</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>391</v>
+      </c>
+      <c r="E14" s="59">
         <v>15</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="7">
+        <v>365</v>
+      </c>
+      <c r="G14" s="59">
         <v>15</v>
       </c>
       <c r="H14" s="8">
@@ -3458,28 +3458,28 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="7">
-        <v>15</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="7">
-        <v>15</v>
-      </c>
-      <c r="H15" s="8">
+      <c r="C15" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E15" s="10">
+        <v>15</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="G15" s="10">
+        <v>15</v>
+      </c>
+      <c r="H15" s="11">
         <v>10</v>
       </c>
     </row>
@@ -3491,16 +3491,16 @@
         <v>0</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>88</v>
+        <v>397</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>89</v>
+        <v>398</v>
       </c>
       <c r="E16" s="5">
         <v>15</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>100</v>
+        <v>367</v>
       </c>
       <c r="G16" s="5">
         <v>15</v>
@@ -3517,16 +3517,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>90</v>
+        <v>399</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>79</v>
+        <v>272</v>
       </c>
       <c r="E17" s="7">
         <v>15</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>100</v>
+        <v>367</v>
       </c>
       <c r="G17" s="7">
         <v>15</v>
@@ -3543,16 +3543,16 @@
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>92</v>
+        <v>381</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>375</v>
       </c>
       <c r="E18" s="7">
         <v>15</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>100</v>
+        <v>367</v>
       </c>
       <c r="G18" s="7">
         <v>15</v>
@@ -3568,17 +3568,17 @@
       <c r="B19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>83</v>
+      <c r="C19" s="59" t="s">
+        <v>59</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>93</v>
+        <v>400</v>
       </c>
       <c r="E19" s="7">
         <v>15</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>101</v>
+        <v>354</v>
       </c>
       <c r="G19" s="7">
         <v>15</v>
@@ -3595,16 +3595,16 @@
         <v>4</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>94</v>
+        <v>377</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="E20" s="7">
         <v>15</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>101</v>
+        <v>354</v>
       </c>
       <c r="G20" s="7">
         <v>15</v>
@@ -3621,16 +3621,16 @@
         <v>21</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>96</v>
+        <v>403</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>97</v>
+        <v>402</v>
       </c>
       <c r="E21" s="7">
         <v>15</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>101</v>
+        <v>354</v>
       </c>
       <c r="G21" s="7">
         <v>15</v>
@@ -3647,16 +3647,16 @@
         <v>22</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>99</v>
+        <v>404</v>
       </c>
       <c r="E22" s="7">
         <v>15</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>102</v>
+        <v>355</v>
       </c>
       <c r="G22" s="7">
         <v>15</v>
@@ -3673,16 +3673,16 @@
         <v>0</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>103</v>
+        <v>405</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>104</v>
+        <v>406</v>
       </c>
       <c r="E23" s="5">
         <v>15</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>116</v>
+        <v>356</v>
       </c>
       <c r="G23" s="5">
         <v>15</v>
@@ -3699,16 +3699,16 @@
         <v>1</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>105</v>
+        <v>407</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>106</v>
+        <v>408</v>
       </c>
       <c r="E24" s="7">
         <v>15</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>116</v>
+        <v>356</v>
       </c>
       <c r="G24" s="7">
         <v>15</v>
@@ -3725,16 +3725,16 @@
         <v>2</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>107</v>
+        <v>409</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>108</v>
+        <v>410</v>
       </c>
       <c r="E25" s="7">
         <v>15</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>116</v>
+        <v>356</v>
       </c>
       <c r="G25" s="7">
         <v>15</v>
@@ -3750,17 +3750,17 @@
       <c r="B26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>109</v>
+      <c r="C26" s="59" t="s">
+        <v>59</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>110</v>
+        <v>411</v>
       </c>
       <c r="E26" s="7">
         <v>15</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>117</v>
+        <v>368</v>
       </c>
       <c r="G26" s="7">
         <v>15</v>
@@ -3777,16 +3777,16 @@
         <v>4</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>111</v>
+        <v>377</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>112</v>
+        <v>412</v>
       </c>
       <c r="E27" s="7">
         <v>15</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>117</v>
+        <v>368</v>
       </c>
       <c r="G27" s="7">
         <v>15</v>
@@ -3803,16 +3803,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>113</v>
+        <v>413</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>114</v>
+        <v>414</v>
       </c>
       <c r="E28" s="7">
         <v>15</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>117</v>
+        <v>368</v>
       </c>
       <c r="G28" s="7">
         <v>15</v>
@@ -3829,16 +3829,16 @@
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>98</v>
+        <v>415</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>115</v>
+        <v>416</v>
       </c>
       <c r="E29" s="7">
         <v>15</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>118</v>
+        <v>369</v>
       </c>
       <c r="G29" s="7">
         <v>15</v>
@@ -3855,16 +3855,16 @@
         <v>0</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>120</v>
+        <v>417</v>
       </c>
       <c r="E30" s="5">
         <v>15</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>131</v>
+        <v>357</v>
       </c>
       <c r="G30" s="5">
         <v>15</v>
@@ -3877,22 +3877,22 @@
       <c r="A31" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="C31" s="59" t="s">
+        <v>418</v>
+      </c>
+      <c r="D31" s="59">
+        <v>1965</v>
+      </c>
+      <c r="E31" s="59">
         <v>15</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G31" s="7">
+        <v>357</v>
+      </c>
+      <c r="G31" s="59">
         <v>15</v>
       </c>
       <c r="H31" s="8">
@@ -3903,22 +3903,22 @@
       <c r="A32" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="7">
+      <c r="C32" s="59" t="s">
+        <v>419</v>
+      </c>
+      <c r="D32" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="E32" s="59">
         <v>15</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G32" s="7">
+        <v>357</v>
+      </c>
+      <c r="G32" s="59">
         <v>15</v>
       </c>
       <c r="H32" s="8">
@@ -3929,22 +3929,22 @@
       <c r="A33" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="C33" s="59" t="s">
+        <v>421</v>
+      </c>
+      <c r="D33" s="59" t="s">
+        <v>422</v>
+      </c>
+      <c r="E33" s="59">
         <v>15</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G33" s="7">
+        <v>358</v>
+      </c>
+      <c r="G33" s="59">
         <v>15</v>
       </c>
       <c r="H33" s="8">
@@ -3955,22 +3955,22 @@
       <c r="A34" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="C34" s="59" t="s">
+        <v>423</v>
+      </c>
+      <c r="D34" s="60" t="s">
+        <v>424</v>
+      </c>
+      <c r="E34" s="59">
         <v>15</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G34" s="7">
+        <v>358</v>
+      </c>
+      <c r="G34" s="59">
         <v>15</v>
       </c>
       <c r="H34" s="8">
@@ -3981,22 +3981,22 @@
       <c r="A35" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="7">
+      <c r="C35" s="59" t="s">
+        <v>425</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>426</v>
+      </c>
+      <c r="E35" s="59">
         <v>15</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G35" s="7">
+        <v>358</v>
+      </c>
+      <c r="G35" s="59">
         <v>15</v>
       </c>
       <c r="H35" s="8">
@@ -4004,28 +4004,28 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="7" t="s">
+      <c r="A36" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E36" s="7">
-        <v>15</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" s="7">
-        <v>15</v>
-      </c>
-      <c r="H36" s="8">
+      <c r="C36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="E36" s="10">
+        <v>15</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="G36" s="10">
+        <v>15</v>
+      </c>
+      <c r="H36" s="11">
         <v>10</v>
       </c>
     </row>
@@ -4037,16 +4037,16 @@
         <v>0</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>137</v>
+        <v>384</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>138</v>
+        <v>428</v>
       </c>
       <c r="E37" s="5">
         <v>15</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>134</v>
+        <v>359</v>
       </c>
       <c r="G37" s="5">
         <v>15</v>
@@ -4062,17 +4062,17 @@
       <c r="B38" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>139</v>
+      <c r="C38" s="59" t="s">
+        <v>429</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>71</v>
+        <v>430</v>
       </c>
       <c r="E38" s="7">
         <v>15</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>134</v>
+        <v>359</v>
       </c>
       <c r="G38" s="7">
         <v>15</v>
@@ -4089,16 +4089,16 @@
         <v>2</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>140</v>
+        <v>431</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>141</v>
+        <v>432</v>
       </c>
       <c r="E39" s="7">
         <v>15</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>134</v>
+        <v>359</v>
       </c>
       <c r="G39" s="7">
         <v>15</v>
@@ -4114,17 +4114,17 @@
       <c r="B40" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>109</v>
+      <c r="C40" s="59" t="s">
+        <v>421</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>142</v>
+        <v>433</v>
       </c>
       <c r="E40" s="7">
         <v>15</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>135</v>
+        <v>371</v>
       </c>
       <c r="G40" s="7">
         <v>15</v>
@@ -4141,16 +4141,16 @@
         <v>4</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>143</v>
+        <v>434</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>144</v>
+        <v>435</v>
       </c>
       <c r="E41" s="7">
         <v>15</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>135</v>
+        <v>371</v>
       </c>
       <c r="G41" s="7">
         <v>15</v>
@@ -4167,16 +4167,16 @@
         <v>21</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>145</v>
+        <v>436</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>146</v>
+        <v>437</v>
       </c>
       <c r="E42" s="7">
         <v>15</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>135</v>
+        <v>371</v>
       </c>
       <c r="G42" s="7">
         <v>15</v>
@@ -4193,16 +4193,16 @@
         <v>22</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>36</v>
+        <v>438</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>147</v>
+        <v>439</v>
       </c>
       <c r="E43" s="10">
         <v>15</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>136</v>
+        <v>360</v>
       </c>
       <c r="G43" s="10">
         <v>15</v>
@@ -4249,7 +4249,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>14</v>
@@ -4258,18 +4258,18 @@
         <v>18</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>435</v>
+        <v>347</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
       <c r="C2" s="5">
         <v>120</v>
@@ -4283,10 +4283,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="C3" s="7">
         <v>120</v>
@@ -4300,10 +4300,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="C4" s="7">
         <v>120</v>
@@ -4317,10 +4317,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>433</v>
+        <v>345</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="C5" s="7">
         <v>120</v>
@@ -4334,10 +4334,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>434</v>
+        <v>346</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>175</v>
+        <v>87</v>
       </c>
       <c r="C6" s="7">
         <v>120</v>
@@ -4351,10 +4351,10 @@
     </row>
     <row r="7" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="C7" s="10">
         <v>120</v>
@@ -4381,7 +4381,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4414,13 +4414,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -4431,16 +4431,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5">
         <v>30</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>66</v>
+        <v>372</v>
       </c>
       <c r="G2" s="5">
         <v>120</v>
@@ -4457,10 +4457,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E3" s="7">
         <v>30</v>
@@ -4479,10 +4479,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E4" s="10">
         <v>30</v>
@@ -4501,16 +4501,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5">
         <v>30</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>66</v>
+        <v>372</v>
       </c>
       <c r="G5" s="5">
         <v>120</v>
@@ -4527,10 +4527,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E6" s="7">
         <v>30</v>
@@ -4549,10 +4549,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E7" s="10">
         <v>30</v>
@@ -4571,16 +4571,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5">
         <v>30</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>66</v>
+        <v>372</v>
       </c>
       <c r="G8" s="5">
         <v>120</v>
@@ -4597,10 +4597,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7">
         <v>30</v>
@@ -4619,10 +4619,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E10" s="10">
         <v>30</v>
@@ -4641,16 +4641,16 @@
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5">
         <v>30</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>66</v>
+        <v>372</v>
       </c>
       <c r="G11" s="5">
         <v>120</v>
@@ -4667,10 +4667,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E12" s="7">
         <v>30</v>
@@ -4689,10 +4689,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E13" s="10">
         <v>30</v>
@@ -4711,16 +4711,16 @@
         <v>0</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E14" s="5">
         <v>30</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>66</v>
+        <v>372</v>
       </c>
       <c r="G14" s="5">
         <v>120</v>
@@ -4737,10 +4737,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E15" s="7">
         <v>30</v>
@@ -4759,10 +4759,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E16" s="10">
         <v>30</v>
@@ -4781,16 +4781,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E17" s="5">
         <v>30</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>66</v>
+        <v>372</v>
       </c>
       <c r="G17" s="5">
         <v>120</v>
@@ -4807,10 +4807,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E18" s="7">
         <v>30</v>
@@ -4829,10 +4829,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E19" s="10">
         <v>30</v>
@@ -4857,7 +4857,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4888,7 +4888,7 @@
         <v>18</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4899,10 +4899,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>308</v>
+        <v>220</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>338</v>
+        <v>250</v>
       </c>
       <c r="E2" s="35">
         <v>60</v>
@@ -4919,10 +4919,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>309</v>
+        <v>221</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>339</v>
+        <v>251</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="38">
@@ -4937,10 +4937,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>310</v>
+        <v>222</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>340</v>
+        <v>252</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="38">
@@ -4955,7 +4955,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>311</v>
+        <v>223</v>
       </c>
       <c r="D5" s="37">
         <v>7</v>
@@ -4973,10 +4973,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>312</v>
+        <v>224</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>341</v>
+        <v>253</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="38">
@@ -4991,10 +4991,10 @@
         <v>21</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>313</v>
+        <v>225</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>342</v>
+        <v>254</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="38">
@@ -5009,10 +5009,10 @@
         <v>22</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>314</v>
+        <v>226</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>343</v>
+        <v>255</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="38">
@@ -5024,13 +5024,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>315</v>
+        <v>227</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>344</v>
+        <v>256</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="38">
@@ -5042,13 +5042,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>316</v>
+        <v>228</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>345</v>
+        <v>257</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="38">
@@ -5060,13 +5060,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>317</v>
+        <v>229</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>346</v>
+        <v>258</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="40">
@@ -5081,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>318</v>
+        <v>230</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>347</v>
+        <v>259</v>
       </c>
       <c r="E12" s="35">
         <v>60</v>
@@ -5101,10 +5101,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>319</v>
+        <v>231</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>348</v>
+        <v>260</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="38">
@@ -5119,10 +5119,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>320</v>
+        <v>232</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>349</v>
+        <v>261</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="38">
@@ -5137,10 +5137,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>321</v>
+        <v>233</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>350</v>
+        <v>262</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="38">
@@ -5155,10 +5155,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>322</v>
+        <v>234</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>351</v>
+        <v>263</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="38">
@@ -5173,10 +5173,10 @@
         <v>21</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>323</v>
+        <v>235</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>352</v>
+        <v>264</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38">
@@ -5191,10 +5191,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>324</v>
+        <v>236</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>353</v>
+        <v>265</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="38">
@@ -5206,13 +5206,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>326</v>
+        <v>238</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>354</v>
+        <v>266</v>
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="38">
@@ -5224,13 +5224,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>325</v>
+        <v>237</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>355</v>
+        <v>267</v>
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="38">
@@ -5242,13 +5242,13 @@
         <v>7</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>327</v>
+        <v>239</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>356</v>
+        <v>268</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="40">
@@ -5263,10 +5263,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>328</v>
+        <v>240</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>357</v>
+        <v>269</v>
       </c>
       <c r="E22" s="35">
         <v>60</v>
@@ -5283,10 +5283,10 @@
         <v>1</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>329</v>
+        <v>241</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>358</v>
+        <v>270</v>
       </c>
       <c r="E23" s="37"/>
       <c r="F23" s="38">
@@ -5301,10 +5301,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>330</v>
+        <v>242</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>359</v>
+        <v>271</v>
       </c>
       <c r="E24" s="37"/>
       <c r="F24" s="38">
@@ -5319,10 +5319,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>393</v>
+        <v>305</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>360</v>
+        <v>272</v>
       </c>
       <c r="E25" s="37"/>
       <c r="F25" s="38">
@@ -5337,10 +5337,10 @@
         <v>4</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>331</v>
+        <v>243</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>361</v>
+        <v>273</v>
       </c>
       <c r="E26" s="37"/>
       <c r="F26" s="38">
@@ -5355,10 +5355,10 @@
         <v>21</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>332</v>
+        <v>244</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>362</v>
+        <v>274</v>
       </c>
       <c r="E27" s="37"/>
       <c r="F27" s="38">
@@ -5373,10 +5373,10 @@
         <v>22</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>333</v>
+        <v>245</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>363</v>
+        <v>275</v>
       </c>
       <c r="E28" s="37"/>
       <c r="F28" s="38">
@@ -5388,13 +5388,13 @@
         <v>8</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>334</v>
+        <v>246</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>364</v>
+        <v>276</v>
       </c>
       <c r="E29" s="37"/>
       <c r="F29" s="38">
@@ -5406,13 +5406,13 @@
         <v>8</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>335</v>
+        <v>247</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>365</v>
+        <v>277</v>
       </c>
       <c r="E30" s="37"/>
       <c r="F30" s="38">
@@ -5424,13 +5424,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>405</v>
+        <v>317</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>394</v>
+        <v>306</v>
       </c>
       <c r="E31" s="39"/>
       <c r="F31" s="40">
@@ -5445,10 +5445,10 @@
         <v>0</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>336</v>
+        <v>248</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>366</v>
+        <v>278</v>
       </c>
       <c r="E32" s="35">
         <v>60</v>
@@ -5465,10 +5465,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>404</v>
+        <v>316</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>367</v>
+        <v>279</v>
       </c>
       <c r="E33" s="37"/>
       <c r="F33" s="38">
@@ -5483,10 +5483,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>406</v>
+        <v>318</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>368</v>
+        <v>280</v>
       </c>
       <c r="E34" s="37"/>
       <c r="F34" s="38">
@@ -5501,10 +5501,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>407</v>
+        <v>319</v>
       </c>
       <c r="D35" s="37" t="s">
-        <v>369</v>
+        <v>281</v>
       </c>
       <c r="E35" s="37"/>
       <c r="F35" s="38">
@@ -5519,10 +5519,10 @@
         <v>4</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>408</v>
+        <v>320</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>370</v>
+        <v>282</v>
       </c>
       <c r="E36" s="37"/>
       <c r="F36" s="38">
@@ -5537,10 +5537,10 @@
         <v>21</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>409</v>
+        <v>321</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>352</v>
+        <v>264</v>
       </c>
       <c r="E37" s="37"/>
       <c r="F37" s="38">
@@ -5555,10 +5555,10 @@
         <v>22</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>410</v>
+        <v>322</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>382</v>
+        <v>294</v>
       </c>
       <c r="E38" s="37"/>
       <c r="F38" s="38">
@@ -5570,13 +5570,13 @@
         <v>9</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>411</v>
+        <v>323</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>371</v>
+        <v>283</v>
       </c>
       <c r="E39" s="37"/>
       <c r="F39" s="38">
@@ -5588,13 +5588,13 @@
         <v>9</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>412</v>
+        <v>324</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>372</v>
+        <v>284</v>
       </c>
       <c r="E40" s="37"/>
       <c r="F40" s="38">
@@ -5606,13 +5606,13 @@
         <v>9</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>413</v>
+        <v>325</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>373</v>
+        <v>285</v>
       </c>
       <c r="E41" s="39"/>
       <c r="F41" s="40">
@@ -5627,10 +5627,10 @@
         <v>0</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>414</v>
+        <v>326</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="E42" s="35">
         <v>60</v>
@@ -5647,10 +5647,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>415</v>
+        <v>327</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>374</v>
+        <v>286</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38">
@@ -5665,10 +5665,10 @@
         <v>2</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>416</v>
+        <v>328</v>
       </c>
       <c r="D44" s="37" t="s">
-        <v>375</v>
+        <v>287</v>
       </c>
       <c r="E44" s="37"/>
       <c r="F44" s="38">
@@ -5683,10 +5683,10 @@
         <v>3</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>417</v>
+        <v>329</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>376</v>
+        <v>288</v>
       </c>
       <c r="E45" s="37"/>
       <c r="F45" s="38">
@@ -5701,10 +5701,10 @@
         <v>4</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>418</v>
+        <v>330</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>377</v>
+        <v>289</v>
       </c>
       <c r="E46" s="37"/>
       <c r="F46" s="38">
@@ -5719,10 +5719,10 @@
         <v>21</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>419</v>
+        <v>331</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>378</v>
+        <v>290</v>
       </c>
       <c r="E47" s="37"/>
       <c r="F47" s="38">
@@ -5737,10 +5737,10 @@
         <v>22</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>420</v>
+        <v>332</v>
       </c>
       <c r="D48" s="37" t="s">
-        <v>379</v>
+        <v>291</v>
       </c>
       <c r="E48" s="37"/>
       <c r="F48" s="38">
@@ -5752,13 +5752,13 @@
         <v>10</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>421</v>
+        <v>333</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>380</v>
+        <v>292</v>
       </c>
       <c r="E49" s="37"/>
       <c r="F49" s="38">
@@ -5770,13 +5770,13 @@
         <v>10</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>422</v>
+        <v>334</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>381</v>
+        <v>293</v>
       </c>
       <c r="E50" s="37"/>
       <c r="F50" s="38">
@@ -5788,13 +5788,13 @@
         <v>10</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C51" s="39" t="s">
-        <v>423</v>
+        <v>335</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>392</v>
+        <v>304</v>
       </c>
       <c r="E51" s="39"/>
       <c r="F51" s="40">
@@ -5809,10 +5809,10 @@
         <v>0</v>
       </c>
       <c r="C52" s="35" t="s">
-        <v>424</v>
+        <v>336</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>383</v>
+        <v>295</v>
       </c>
       <c r="E52" s="35">
         <v>60</v>
@@ -5829,10 +5829,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="37" t="s">
-        <v>425</v>
+        <v>337</v>
       </c>
       <c r="D53" s="37" t="s">
-        <v>384</v>
+        <v>296</v>
       </c>
       <c r="E53" s="37"/>
       <c r="F53" s="38">
@@ -5847,10 +5847,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="37" t="s">
-        <v>426</v>
+        <v>338</v>
       </c>
       <c r="D54" s="37" t="s">
-        <v>391</v>
+        <v>303</v>
       </c>
       <c r="E54" s="37"/>
       <c r="F54" s="38">
@@ -5865,7 +5865,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="37" t="s">
-        <v>427</v>
+        <v>339</v>
       </c>
       <c r="D55" s="37">
         <v>6</v>
@@ -5883,10 +5883,10 @@
         <v>4</v>
       </c>
       <c r="C56" s="37" t="s">
-        <v>428</v>
+        <v>340</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>385</v>
+        <v>297</v>
       </c>
       <c r="E56" s="37"/>
       <c r="F56" s="38">
@@ -5901,10 +5901,10 @@
         <v>21</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>429</v>
+        <v>341</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>386</v>
+        <v>298</v>
       </c>
       <c r="E57" s="37"/>
       <c r="F57" s="38">
@@ -5919,10 +5919,10 @@
         <v>22</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>387</v>
+        <v>299</v>
       </c>
       <c r="E58" s="37"/>
       <c r="F58" s="38">
@@ -5934,13 +5934,13 @@
         <v>11</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>388</v>
+        <v>300</v>
       </c>
       <c r="E59" s="37"/>
       <c r="F59" s="38">
@@ -5952,13 +5952,13 @@
         <v>11</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>432</v>
+        <v>344</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>389</v>
+        <v>301</v>
       </c>
       <c r="E60" s="37"/>
       <c r="F60" s="38">
@@ -5970,13 +5970,13 @@
         <v>11</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C61" s="39" t="s">
-        <v>337</v>
+        <v>249</v>
       </c>
       <c r="D61" s="39" t="s">
-        <v>390</v>
+        <v>302</v>
       </c>
       <c r="E61" s="39"/>
       <c r="F61" s="40">
@@ -6025,10 +6025,10 @@
         <v>18</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -6036,10 +6036,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>153</v>
+        <v>65</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="D2" s="26">
         <v>30</v>
@@ -6056,10 +6056,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>396</v>
+        <v>308</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="D3" s="48">
         <v>30</v>
@@ -6076,10 +6076,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>397</v>
+        <v>309</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="D4" s="48">
         <v>30</v>
@@ -6096,10 +6096,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>398</v>
+        <v>310</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="D5" s="48">
         <v>30</v>
@@ -6116,10 +6116,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>399</v>
+        <v>311</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="D6" s="48">
         <v>30</v>
@@ -6136,10 +6136,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>400</v>
+        <v>312</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="D7" s="48">
         <v>30</v>
@@ -6156,10 +6156,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>401</v>
+        <v>313</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="D8" s="48">
         <v>30</v>
@@ -6173,13 +6173,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="D9" s="48">
         <v>30</v>
@@ -6193,13 +6193,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>402</v>
+        <v>314</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>163</v>
+        <v>75</v>
       </c>
       <c r="D10" s="48">
         <v>30</v>
@@ -6213,13 +6213,13 @@
     </row>
     <row r="11" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>403</v>
+        <v>315</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="D11" s="48">
         <v>30</v>
@@ -6233,13 +6233,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="D12" s="48">
         <v>30</v>
@@ -6253,13 +6253,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>166</v>
+        <v>78</v>
       </c>
       <c r="D13" s="48">
         <v>30</v>
@@ -6273,13 +6273,13 @@
     </row>
     <row r="14" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>395</v>
+        <v>307</v>
       </c>
       <c r="D14" s="48">
         <v>30</v>
@@ -6293,13 +6293,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D15" s="48">
         <v>30</v>
@@ -6313,13 +6313,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D16" s="48">
         <v>30</v>
@@ -6333,13 +6333,13 @@
     </row>
     <row r="17" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D17" s="29">
         <v>30</v>

</xml_diff>